<commit_message>
Add New Roles: Swooper
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Among Us code\TheOtherUs-Fix2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA3D2FC-0660-43BB-B44E-1598719A02F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C31BF7-13EB-4019-A3C0-9A8A6490F832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="292">
   <si>
     <t>English</t>
   </si>
@@ -451,9 +451,6 @@
     <t>HandcuffText</t>
   </si>
   <si>
-    <t>戴上手铐</t>
-  </si>
-  <si>
     <t>PlacePortalText</t>
   </si>
   <si>
@@ -479,9 +476,6 @@
   </si>
   <si>
     <t>PlaceTrapText</t>
-  </si>
-  <si>
-    <t>布下陷阱</t>
   </si>
   <si>
     <t>BrainwashText</t>
@@ -726,10 +720,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>罗望子色</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>黏液绿</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -833,9 +823,6 @@
     <t>鮭魚色</t>
   </si>
   <si>
-    <t>波爾多酒紅</t>
-  </si>
-  <si>
     <t>橄欖綠</t>
   </si>
   <si>
@@ -879,9 +866,6 @@
   </si>
   <si>
     <t>軍綠色</t>
-  </si>
-  <si>
-    <t>羅望子色</t>
   </si>
   <si>
     <t>紫紅色</t>
@@ -978,6 +962,34 @@
   </si>
   <si>
     <t>尝试击杀被保护玩家</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>罗望子</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>羅望子</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>波爾多</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>minerText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>挖洞</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>上铐</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>布下陷阱</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1577,8 +1589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1332"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.875" defaultRowHeight="14.25"/>
@@ -1647,7 +1659,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>17</v>
@@ -1658,68 +1670,68 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>184</v>
-      </c>
       <c r="O3" s="5" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="28.5">
       <c r="A5" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="O5" s="5" t="s">
         <v>281</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="71.25">
@@ -1727,43 +1739,43 @@
         <v>19</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="71.25">
       <c r="A10" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="O10" s="6" t="s">
         <v>275</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="28.5">
       <c r="A11" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>181</v>
-      </c>
       <c r="O11" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="5" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -5748,7 +5760,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.875" defaultRowHeight="18" customHeight="1"/>
@@ -5831,13 +5843,13 @@
         <v>25</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="O2" s="7" t="s">
         <v>26</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="14.25">
@@ -5848,13 +5860,13 @@
         <v>28</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>249</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="14.25">
@@ -5865,13 +5877,13 @@
         <v>30</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="14.25">
@@ -5882,13 +5894,13 @@
         <v>32</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="O5" s="7" t="s">
         <v>33</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="14.25">
@@ -5899,13 +5911,13 @@
         <v>35</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="O6" s="7" t="s">
         <v>36</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="14.25">
@@ -5916,13 +5928,13 @@
         <v>38</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O7" s="7" t="s">
         <v>39</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="14.25">
@@ -5933,13 +5945,13 @@
         <v>41</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="14.25">
@@ -5950,13 +5962,13 @@
         <v>43</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>44</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="14.25">
@@ -5967,13 +5979,13 @@
         <v>46</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="14.25">
@@ -5984,13 +5996,13 @@
         <v>48</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>49</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="14.25">
@@ -6001,13 +6013,13 @@
         <v>51</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="O12" s="7" t="s">
         <v>52</v>
       </c>
       <c r="P12" s="7" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="14.25">
@@ -6018,13 +6030,13 @@
         <v>54</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="O13" s="7" t="s">
         <v>55</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="14.25">
@@ -6035,13 +6047,13 @@
         <v>57</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="O14" s="7" t="s">
         <v>58</v>
       </c>
       <c r="P14" s="7" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="14.25">
@@ -6052,13 +6064,13 @@
         <v>60</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="O15" s="7" t="s">
         <v>61</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="14.25">
@@ -6069,13 +6081,13 @@
         <v>63</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="O16" s="7" t="s">
         <v>64</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="14.25">
@@ -6086,13 +6098,13 @@
         <v>66</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="O17" s="7" t="s">
         <v>67</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="14.25">
@@ -6103,166 +6115,166 @@
         <v>69</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="O18" s="7" t="s">
         <v>70</v>
       </c>
       <c r="P18" s="7" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="14.25">
       <c r="A19" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="14.25">
       <c r="A20" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="O20" s="7" t="s">
-        <v>216</v>
+        <v>285</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>265</v>
+        <v>286</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="14.25">
       <c r="A21" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="O21" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="14.25">
       <c r="A22" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="P22" s="7" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="14.25">
       <c r="A23" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="14.25">
       <c r="A24" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="P24" s="7" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="14.25">
       <c r="A25" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="O25" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="14.25">
       <c r="A26" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="P26" s="7" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="14.25">
       <c r="A27" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P27" s="7" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -6274,10 +6286,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Q57"/>
+  <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="O61" sqref="O61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
@@ -7185,46 +7197,46 @@
       <c r="B35" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O35" s="4" t="s">
-        <v>137</v>
+      <c r="O35" s="7" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="36" spans="1:17">
       <c r="A36" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O36" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:17">
       <c r="A37" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O37" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:17">
       <c r="A38" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O38" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>21</v>
@@ -7235,7 +7247,7 @@
     </row>
     <row r="40" spans="1:17">
       <c r="A40" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>21</v>
@@ -7246,189 +7258,200 @@
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O41" s="4" t="s">
-        <v>147</v>
+      <c r="O41" s="7" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="42" spans="1:17">
       <c r="A42" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O42" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:17">
       <c r="A43" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:17">
       <c r="A44" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="45" spans="1:17">
       <c r="A45" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:17">
       <c r="A46" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:17">
       <c r="A47" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:17">
       <c r="A48" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:15">
       <c r="A50" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:15">
       <c r="A52" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:15">
       <c r="A53" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="1:15">
       <c r="A54" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:15">
       <c r="A55" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:15">
       <c r="A56" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O57" s="1" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
+      <c r="A58" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O58" s="7" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bugs and restore old Snitch
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Among Us code\TheOtherUs-Beta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D818B83-BC16-42AA-B62C-92833344DA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A446AA3A-6B59-4D6D-BA75-166115F0D29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -713,437 +713,437 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;size=75%&gt;Mod修改：&lt;color=#FFB793&gt;沫夏悠轩&lt;/color&gt;&amp;&lt;color=#FCCE03FF&gt;善良的好人&lt;/color&gt;
-&lt;color=#FCCE03FF&gt;天寸梦初&lt;/color&gt;&amp;&lt;color=#FCCE03FF&gt;Imp11&lt;/color&gt;
+    <t xml:space="preserve">&lt;size=110%&gt;&lt;color=#ff351f&gt;我们的超多职业&lt;/color&gt;&lt;/size&gt; </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;size=130%&gt;&lt;color=#ff351f&gt;我们的超多职业&lt;/color&gt;&lt;/size&gt; </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Credits</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOU Credits</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>English</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>模组贡献者</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>安装星门</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlaceJackInTheBoxText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>jackalSidekickText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>招募</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>killButtonText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>击杀</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>VampireText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HandcuffText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShieldText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>doomsayerText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>揭示</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>AkujoHonmeiText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>AkujoBackupText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShiftText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>SampleText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>hackerVitalText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命检测仪</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>hackerDoorLogText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>日志</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>bodyGuardText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>保护</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>观察</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PrivateInvestigatorWatchText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GarlicText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>放置大蒜</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>usePortalText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>SwoopText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>隐身</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>CurseText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>EraserText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>点灯</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>CleanText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>DragBodyText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>VultureText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>RememberText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>回忆</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>监控</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>CamButtonText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>DouseText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PursuerText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>WitchText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>诅咒</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">下咒 </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>CurseKillText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>标记/传送</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>传送</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>jumperText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>jumperJumpText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>NinjaText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>刺杀</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>BlackmailerText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>MayorButtonText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>紧急会议</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ConvertText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>放置陷阱</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>trapperTrapText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TerroristBombText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>放置炸弹</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>AdminMapText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理地图</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>LighterText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>hackerButtonText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑入</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>defuseBombText</t>
+  </si>
+  <si>
+    <t>拆弹</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TimeShieldText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>AlertText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>SeerText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>buttonBarryText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>DisperseText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>分散</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>prophetMeetingButton</t>
+  </si>
+  <si>
+    <t>The Prophet can't start an emergency meeting</t>
+  </si>
+  <si>
+    <t>预言家不可以发起紧急会议</t>
+  </si>
+  <si>
+    <t>swapperMeetingButton</t>
+  </si>
+  <si>
+    <t>The Swapper can't start an emergency meeting</t>
+  </si>
+  <si>
+    <t>スワッパーはミーティングを招集できない</t>
+  </si>
+  <si>
+    <t>换票师不可以发起紧急会议</t>
+  </si>
+  <si>
+    <t>jesterMeetingButton</t>
+  </si>
+  <si>
+    <t>The Jester can't start an emergency meeting</t>
+  </si>
+  <si>
+    <t>ジェスターはミーティングを招集できない</t>
+  </si>
+  <si>
+    <t>小丑不可以发起紧急会议</t>
+  </si>
+  <si>
+    <t>lawyerMeetingButton</t>
+  </si>
+  <si>
+    <t>The Lawyer can't start an emergency meeting</t>
+  </si>
+  <si>
+    <t>弁護士はミーティングを招集できない</t>
+  </si>
+  <si>
+    <t>律师不可以发起紧急会议</t>
+  </si>
+  <si>
+    <t>fortuneTellerMeetingButton</t>
+  </si>
+  <si>
+    <t>The Fortune Teller can't start an emergency meeting</t>
+  </si>
+  <si>
+    <t>占卜师不可以发起紧急会议</t>
+  </si>
+  <si>
+    <t>ProsecutorMeetingButton</t>
+  </si>
+  <si>
+    <t>The Prosecutor can't start an emergency meeting</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>处刑者不可以发起紧急会议</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>meetingCount</t>
+  </si>
+  <si>
+    <t>{0} and the ship has {1}</t>
+  </si>
+  <si>
+    <t>{0}と船に{1}がいます</t>
+  </si>
+  <si>
+    <t>{0}次，全船剩余{1}次</t>
+  </si>
+  <si>
+    <t>放置</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TricksterPlaceText1</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>自爆</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TricksterPlaceText2</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>YOU ARE BLACKMAILED</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>BlackmailShhhText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>嘘！不许说话！</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=75%&gt;Mod修改：&lt;color=#FFB793&gt;沫夏悠轩&lt;/color&gt; &amp; &lt;color=#FCCE03FF&gt;善良的好人&lt;/color&gt;
+&lt;color=#FCCE03FF&gt;天寸梦初&lt;/color&gt; &amp; &lt;color=#FCCE03FF&gt;Imp11&lt;/color&gt;
 美工: &lt;color=#00FFFFFF&gt;方块&lt;/color&gt;&lt;/size&gt;
 &lt;size=70%&gt;基于TheOtherUs&lt;/size&gt;</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;size=75%&gt;Mod修改: &lt;color=#FFB793&gt;沫夏悠轩&lt;/color&gt;&amp;&lt;color=#FCCE03FF&gt;善良的好人&lt;/color&gt;
-&lt;color=#FCCE03FF&gt;天寸梦初&lt;/color&gt;&amp;&lt;color=#FCCE03FF&gt;Imp11&lt;/color&gt;
+    <t>&lt;size=75%&gt;Mod修改: &lt;color=#FFB793&gt;沫夏悠轩&lt;/color&gt; &amp; &lt;color=#FCCE03FF&gt;善良的好人&lt;/color&gt;
+&lt;color=#FCCE03FF&gt;天寸梦初&lt;/color&gt; &amp; &lt;color=#FCCE03FF&gt;Imp11&lt;/color&gt;
 美工: &lt;color=#00FFFFFF&gt;方块&lt;/color&gt;&lt;/size&gt;
 &lt;size=70%&gt;基于TheOtherUs&lt;/size&gt;</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;size=110%&gt;&lt;color=#ff351f&gt;我们的超多职业&lt;/color&gt;&lt;/size&gt; </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;size=130%&gt;&lt;color=#ff351f&gt;我们的超多职业&lt;/color&gt;&lt;/size&gt; </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Credits</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TOU Credits</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>English</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>模组贡献者</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>安装星门</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>PlaceJackInTheBoxText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>jackalSidekickText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>招募</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>killButtonText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>击杀</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>VampireText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>HandcuffText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ShieldText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>doomsayerText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>揭示</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>AkujoHonmeiText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>AkujoBackupText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ShiftText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>SampleText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>hackerVitalText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>生命检测仪</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>hackerDoorLogText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>日志</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>bodyGuardText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>保护</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>观察</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>PrivateInvestigatorWatchText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GarlicText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>放置大蒜</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>usePortalText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>SwoopText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>隐身</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>CurseText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>EraserText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>点灯</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>CleanText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>DragBodyText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>VultureText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>RememberText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>回忆</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>监控</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>CamButtonText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>DouseText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>PursuerText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>WitchText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>诅咒</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">下咒 </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>CurseKillText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>标记/传送</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>传送</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>jumperText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>jumperJumpText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>NinjaText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>刺杀</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>BlackmailerText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>MayorButtonText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>紧急会议</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ConvertText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>放置陷阱</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>trapperTrapText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TerroristBombText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>放置炸弹</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>AdminMapText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>管理地图</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>LighterText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>hackerButtonText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>黑入</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>defuseBombText</t>
-  </si>
-  <si>
-    <t>拆弹</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TimeShieldText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>AlertText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>SeerText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>buttonBarryText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>DisperseText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>分散</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>prophetMeetingButton</t>
-  </si>
-  <si>
-    <t>The Prophet can't start an emergency meeting</t>
-  </si>
-  <si>
-    <t>预言家不可以发起紧急会议</t>
-  </si>
-  <si>
-    <t>swapperMeetingButton</t>
-  </si>
-  <si>
-    <t>The Swapper can't start an emergency meeting</t>
-  </si>
-  <si>
-    <t>スワッパーはミーティングを招集できない</t>
-  </si>
-  <si>
-    <t>换票师不可以发起紧急会议</t>
-  </si>
-  <si>
-    <t>jesterMeetingButton</t>
-  </si>
-  <si>
-    <t>The Jester can't start an emergency meeting</t>
-  </si>
-  <si>
-    <t>ジェスターはミーティングを招集できない</t>
-  </si>
-  <si>
-    <t>小丑不可以发起紧急会议</t>
-  </si>
-  <si>
-    <t>lawyerMeetingButton</t>
-  </si>
-  <si>
-    <t>The Lawyer can't start an emergency meeting</t>
-  </si>
-  <si>
-    <t>弁護士はミーティングを招集できない</t>
-  </si>
-  <si>
-    <t>律师不可以发起紧急会议</t>
-  </si>
-  <si>
-    <t>fortuneTellerMeetingButton</t>
-  </si>
-  <si>
-    <t>The Fortune Teller can't start an emergency meeting</t>
-  </si>
-  <si>
-    <t>占卜师不可以发起紧急会议</t>
-  </si>
-  <si>
-    <t>ProsecutorMeetingButton</t>
-  </si>
-  <si>
-    <t>The Prosecutor can't start an emergency meeting</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>处刑者不可以发起紧急会议</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>meetingCount</t>
-  </si>
-  <si>
-    <t>{0} and the ship has {1}</t>
-  </si>
-  <si>
-    <t>{0}と船に{1}がいます</t>
-  </si>
-  <si>
-    <t>{0}次，全船剩余{1}次</t>
-  </si>
-  <si>
-    <t>放置</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TricksterPlaceText1</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>自爆</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TricksterPlaceText2</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>YOU ARE BLACKMAILED</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>BlackmailShhhText</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>嘘！不许说话！</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1756,7 +1756,7 @@
   <dimension ref="A1:Q1333"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.875" defaultRowHeight="14.25"/>
@@ -1772,7 +1772,7 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="B1" s="12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1842,7 +1842,7 @@
         <v>148</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1853,7 +1853,7 @@
         <v>193</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="28.5">
@@ -1902,13 +1902,13 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="O9" s="12" t="s">
         <v>208</v>
-      </c>
-      <c r="O9" s="12" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="71.25">
@@ -1919,7 +1919,7 @@
         <v>190</v>
       </c>
       <c r="O10" s="11" t="s">
-        <v>204</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="71.25">
@@ -1930,7 +1930,7 @@
         <v>187</v>
       </c>
       <c r="O11" s="11" t="s">
-        <v>203</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="28.5">
@@ -1977,10 +1977,10 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="13" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1993,19 +1993,19 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="13" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2018,19 +2018,19 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="13" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2043,19 +2043,19 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2070,15 +2070,15 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="13" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2093,15 +2093,15 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="13" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2116,7 +2116,7 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -2124,10 +2124,10 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2140,11 +2140,11 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -2152,13 +2152,13 @@
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B25" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="O25" s="12" t="s">
         <v>313</v>
-      </c>
-      <c r="O25" s="12" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -6479,8 +6479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S82"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X39" sqref="X39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
@@ -6583,7 +6583,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>21</v>
@@ -6633,7 +6633,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>21</v>
@@ -6651,14 +6651,14 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>21</v>
@@ -6683,7 +6683,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>21</v>
@@ -6708,7 +6708,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>21</v>
@@ -6733,7 +6733,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>21</v>
@@ -6751,7 +6751,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -6830,7 +6830,7 @@
       </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -6910,7 +6910,7 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>21</v>
@@ -6928,7 +6928,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
@@ -6985,7 +6985,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>21</v>
@@ -7010,7 +7010,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>21</v>
@@ -7035,7 +7035,7 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>21</v>
@@ -7060,7 +7060,7 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>21</v>
@@ -7110,7 +7110,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>21</v>
@@ -7185,7 +7185,7 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>21</v>
@@ -7210,7 +7210,7 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>21</v>
@@ -7285,7 +7285,7 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>21</v>
@@ -7310,7 +7310,7 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>21</v>
@@ -7328,14 +7328,14 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>21</v>
@@ -7353,7 +7353,7 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
@@ -7385,7 +7385,7 @@
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>21</v>
@@ -7462,7 +7462,7 @@
     </row>
     <row r="42" spans="1:17">
       <c r="A42" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>21</v>
@@ -7473,7 +7473,7 @@
     </row>
     <row r="43" spans="1:17">
       <c r="A43" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>21</v>
@@ -7506,7 +7506,7 @@
     </row>
     <row r="46" spans="1:17">
       <c r="A46" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>21</v>
@@ -7539,7 +7539,7 @@
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>21</v>
@@ -7550,7 +7550,7 @@
     </row>
     <row r="50" spans="1:15">
       <c r="A50" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>21</v>
@@ -7583,29 +7583,29 @@
     </row>
     <row r="53" spans="1:15">
       <c r="A53" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="54" spans="1:15">
       <c r="A54" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="55" spans="1:15">
       <c r="A55" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>21</v>
@@ -7638,225 +7638,225 @@
     </row>
     <row r="58" spans="1:15">
       <c r="A58" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="59" spans="1:15">
       <c r="A59" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="60" spans="1:15">
       <c r="A60" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="61" spans="1:15">
       <c r="A61" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O61" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="62" spans="1:15">
       <c r="A62" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="63" spans="1:15">
       <c r="A63" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:15">
       <c r="A64" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O64" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:17">
       <c r="A65" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O65" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="66" spans="1:17">
       <c r="A66" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O66" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="67" spans="1:17">
       <c r="A67" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="68" spans="1:17">
       <c r="A68" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="69" spans="1:17">
       <c r="A69" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="70" spans="1:17">
       <c r="A70" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O70" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="71" spans="1:17">
       <c r="A71" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O71" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="72" spans="1:17">
       <c r="A72" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O72" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="73" spans="1:17">
       <c r="A73" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O73" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q73" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="74" spans="1:17">
       <c r="A74" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O74" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="75" spans="1:17">
       <c r="A75" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O75" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="76" spans="1:17">
       <c r="A76" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O76" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="77" spans="1:17">
       <c r="A77" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O77" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="78" spans="1:17">
@@ -7872,29 +7872,29 @@
     </row>
     <row r="79" spans="1:17">
       <c r="A79" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O79" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="80" spans="1:17">
       <c r="A80" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O80" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="82" spans="19:19">
       <c r="S82" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update translation and fix bugs
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Among Us code\TheOtherUs\TheOtherUs-Edited\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD56550-8824-4068-8C67-0BF14FC98B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724E1D0E-2593-4404-9211-5F26B87748A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Button Text" sheetId="8" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Text!$O$1:$O$1117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Text!$O$1:$O$1143</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="691">
   <si>
     <t>English</t>
   </si>
@@ -1654,14 +1654,6 @@
   </si>
   <si>
     <t>最大附加职业数</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>OFF</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ON</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -2030,14 +2022,6 @@
   </si>
   <si>
     <t>预设</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;color=#CCCCCC&gt;关闭&lt;/color&gt;</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;color=#FFFF00&gt;开启&lt;/color&gt;</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -2314,11 +2298,328 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;color=#FFFF00&gt;On&lt;/color&gt;</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;color=#CCCCCC&gt;Off&lt;/color&gt;</t>
+    <t>optionOn</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>optionOff</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Very Short</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>非常短</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>KillDistancesVeryShort</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>船员阵营</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>中立阵营</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>伪装者阵营</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>附加能力</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modifiers</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Impostor Roles</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Neutral Roles</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crewmate Roles</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>CrewmateRolesText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeutralRolesText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ImpostorRolesText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ModifiersText</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>(Use scroll wheel if necessary)\n\n</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>(如有必要，请使用滚轮)\n\n</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>\n Press TAB or Page Number for more... ({0}/{1})</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>useScrollWheel</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>\n 按Tab键查看更多... ({0}/{1})</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pressTabForMore</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Page 1: Vanilla Settings \n\n</t>
+  </si>
+  <si>
+    <t>Page 1: バニラの設定 ￤バニラの設定</t>
+  </si>
+  <si>
+    <t>第一页：游戏设置 \n\n</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Page 1: Hide N Seek Settings \n\n</t>
+  </si>
+  <si>
+    <t>Page 2: Hide N Seek Role Settings \n\n</t>
+  </si>
+  <si>
+    <t>PropHuntPage</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>第1页: 道具躲猫猫模式设置 \n\n</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>第1页：躲猫猫模式设置 \n\n</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>第2页：躲猫猫职业设置 \n\n</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>hideNSeekPage2</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>hideNSeekPage1</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Page 1: Prop Hunt Settings \n\n</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>page1</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>page6</t>
+  </si>
+  <si>
+    <t>page7</t>
+  </si>
+  <si>
+    <t>第2页: 超多职业模组设置 \n</t>
+  </si>
+  <si>
+    <t>第3页: 职业和附加职业设置 \n</t>
+  </si>
+  <si>
+    <t>第4页: 伪装者职业设置 \n</t>
+  </si>
+  <si>
+    <t>第5页: 中立职业设置 \n</t>
+  </si>
+  <si>
+    <t>第6页: 船员职业设置 \n</t>
+  </si>
+  <si>
+    <t>第7页: 附加职业设置 \n</t>
+  </si>
+  <si>
+    <t>Page 2: The Other Us Settings \n</t>
+  </si>
+  <si>
+    <t>Page 3: Role and Modifier Rates \n</t>
+  </si>
+  <si>
+    <t>Page 4: Impostor Role Settings \n</t>
+  </si>
+  <si>
+    <t>Page 5: Neutral Role Settings \n</t>
+  </si>
+  <si>
+    <t>Page 6: Crewmate Role Settings \n</t>
+  </si>
+  <si>
+    <t>Page 7: Modifier Settings \n</t>
+  </si>
+  <si>
+    <t>附加职业</t>
+  </si>
+  <si>
+    <t>Impostors</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Neutrals</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crewmates</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>crewmateRoles</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>neutralRoles</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>impostorRoles</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>modifiers</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>page2</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>page3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>page4</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>page5</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>theOtherRolesSettings</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>模组设置</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>hideNSeekSettings</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>躲猫猫模式设置</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>道具躲猫猫模式设置</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PropHuntSettings</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prop Hunt Settings</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hide 'N Seek Settings</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Other Us Settings</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>theOtherUsSettings</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>guesserSettings</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>impostorRolesSettings</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>neutralRolesSettings</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>crewmateRolesSettings</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>modifierSettings</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>赌怪模式设置</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>伪装者职业设置</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>中立职业设置</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>船员职业设置</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>附加职业设置</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;color=#CCCCCCFF&gt;Off&lt;/color&gt;</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;color=#FFFF00FF&gt;On&lt;/color&gt;</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;color=#FFFF00FF&gt;开启&lt;/color&gt;</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;color=#CCCCCCFF&gt;关闭&lt;/color&gt;</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -2933,10 +3234,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q1414"/>
+  <dimension ref="A1:Q1440"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="O65" sqref="O65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.875" defaultRowHeight="24.95" customHeight="1"/>
@@ -3019,10 +3320,10 @@
         <v>140</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="24.95" customHeight="1">
@@ -3030,10 +3331,10 @@
         <v>142</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="28.5">
@@ -3099,7 +3400,7 @@
         <v>182</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="42.75">
@@ -3110,7 +3411,7 @@
         <v>300</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="42.75">
@@ -3126,10 +3427,10 @@
     </row>
     <row r="13" spans="1:17" ht="313.5">
       <c r="A13" s="7" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -3144,7 +3445,7 @@
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="O13" s="8" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="24.95" customHeight="1">
@@ -3152,1695 +3453,1941 @@
     </row>
     <row r="15" spans="1:17" ht="24.95" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="24.95" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="24.95" customHeight="1">
       <c r="A17" s="7" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="O17" s="8" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="24.95" customHeight="1">
       <c r="A18" s="7" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="24.95" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="O19" s="8" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="24.95" customHeight="1">
       <c r="A20" s="7" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="O20" s="8" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="24.95" customHeight="1">
       <c r="A21" s="7" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="O21" s="8" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="24.95" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="O22" s="8" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="24.95" customHeight="1">
       <c r="A23" s="7" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="O23" s="8" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="24.95" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="O24" s="8" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="24.95" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="O25" s="8" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="24.95" customHeight="1">
       <c r="A26" s="7" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>554</v>
-      </c>
+        <v>550</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="O27" s="8"/>
     </row>
     <row r="28" spans="1:15" ht="24.95" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>581</v>
+        <v>627</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>580</v>
+        <v>624</v>
       </c>
       <c r="O28" s="8" t="s">
-        <v>579</v>
+        <v>626</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="24.95" customHeight="1">
       <c r="A29" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="O29" s="6" t="s">
-        <v>188</v>
+        <v>625</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>622</v>
+      </c>
+      <c r="O29" s="8" t="s">
+        <v>623</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
+      <c r="A30" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>607</v>
+      </c>
+      <c r="O30" s="8" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="31" spans="1:15" ht="24.95" customHeight="1">
       <c r="A31" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7" t="s">
-        <v>274</v>
+        <v>667</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>675</v>
+      </c>
+      <c r="O31" s="8" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="24.95" customHeight="1">
       <c r="A32" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7" t="s">
-        <v>278</v>
+        <v>669</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>674</v>
+      </c>
+      <c r="O32" s="8" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="24.95" customHeight="1">
       <c r="A33" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7" t="s">
-        <v>282</v>
+        <v>672</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>673</v>
+      </c>
+      <c r="O33" s="8" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A34" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="7" t="s">
-        <v>285</v>
-      </c>
+      <c r="A34" s="7"/>
+      <c r="B34" s="8"/>
+      <c r="O34" s="8"/>
     </row>
     <row r="35" spans="1:15" ht="24.95" customHeight="1">
       <c r="A35" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="7"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="7" t="s">
-        <v>270</v>
+        <v>618</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>617</v>
+      </c>
+      <c r="O35" s="8" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="24.95" customHeight="1">
       <c r="A36" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7" t="s">
-        <v>288</v>
+        <v>619</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>616</v>
+      </c>
+      <c r="O36" s="8" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O37" s="6"/>
+      <c r="A37" s="7" t="s">
+        <v>620</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>615</v>
+      </c>
+      <c r="O37" s="8" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="38" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A38" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7" t="s">
-        <v>292</v>
+      <c r="A38" s="8" t="s">
+        <v>621</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>614</v>
+      </c>
+      <c r="O38" s="8" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
-      <c r="O39" s="7"/>
+      <c r="O39" s="6"/>
     </row>
     <row r="40" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A40" s="7" t="s">
-        <v>448</v>
-      </c>
-      <c r="B40" s="7" t="s">
+      <c r="A40" s="8" t="s">
+        <v>661</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>656</v>
+      </c>
+      <c r="O40" s="8" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A41" s="8" t="s">
+        <v>660</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>657</v>
+      </c>
+      <c r="O41" s="8" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A42" s="8" t="s">
+        <v>659</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>658</v>
+      </c>
+      <c r="O42" s="8" t="s">
         <v>610</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A41" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>609</v>
-      </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="7" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A42" s="7" t="s">
-        <v>450</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7" t="s">
-        <v>332</v>
-      </c>
-      <c r="N42" s="7"/>
-      <c r="O42" s="7" t="s">
-        <v>542</v>
-      </c>
     </row>
     <row r="43" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A43" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="O43" s="7" t="s">
-        <v>330</v>
+      <c r="A43" s="8" t="s">
+        <v>662</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>614</v>
+      </c>
+      <c r="O43" s="8" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A44" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="O44" s="7" t="s">
-        <v>307</v>
-      </c>
+      <c r="A44" s="8"/>
     </row>
     <row r="45" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A45" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="7"/>
+      <c r="A45" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="M45" s="6" t="s">
+        <v>629</v>
+      </c>
       <c r="O45" s="7" t="s">
-        <v>308</v>
+        <v>630</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A46" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="7" t="s">
-        <v>309</v>
+      <c r="A46" s="8" t="s">
+        <v>663</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="O46" s="9" t="s">
+        <v>643</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A47" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
-      <c r="M47" s="7"/>
-      <c r="N47" s="7"/>
-      <c r="O47" s="7" t="s">
-        <v>312</v>
+      <c r="A47" s="8" t="s">
+        <v>664</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>650</v>
+      </c>
+      <c r="O47" s="9" t="s">
+        <v>644</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A48" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
-      <c r="N48" s="7"/>
-      <c r="O48" s="7" t="s">
-        <v>321</v>
+      <c r="A48" s="8" t="s">
+        <v>665</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="O48" s="9" t="s">
+        <v>645</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A49" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="7"/>
-      <c r="M49" s="7"/>
-      <c r="N49" s="7"/>
-      <c r="O49" s="7" t="s">
-        <v>322</v>
+      <c r="A49" s="8" t="s">
+        <v>666</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="O49" s="9" t="s">
+        <v>646</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="24.95" customHeight="1">
       <c r="A50" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="7"/>
-      <c r="L50" s="7"/>
-      <c r="M50" s="7"/>
-      <c r="N50" s="7"/>
-      <c r="O50" s="7" t="s">
-        <v>323</v>
+        <v>641</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="O50" s="9" t="s">
+        <v>647</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="24.95" customHeight="1">
       <c r="A51" s="7" t="s">
-        <v>326</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="7" t="s">
-        <v>324</v>
+        <v>642</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="O51" s="9" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="24.95" customHeight="1">
       <c r="A52" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="7"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="7"/>
+        <v>638</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>631</v>
+      </c>
       <c r="O52" s="7" t="s">
-        <v>325</v>
+        <v>635</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O53" s="6"/>
+      <c r="A53" s="7" t="s">
+        <v>637</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="O53" s="7" t="s">
+        <v>636</v>
+      </c>
     </row>
     <row r="54" spans="1:15" ht="24.95" customHeight="1">
       <c r="A54" s="7" t="s">
-        <v>339</v>
+        <v>633</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>334</v>
+        <v>639</v>
       </c>
       <c r="O54" s="7" t="s">
-        <v>333</v>
+        <v>634</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A55" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="O55" s="7" t="s">
-        <v>336</v>
-      </c>
+      <c r="O55" s="6"/>
     </row>
     <row r="56" spans="1:15" ht="24.95" customHeight="1">
       <c r="A56" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="O56" s="7" t="s">
-        <v>340</v>
+        <v>676</v>
+      </c>
+      <c r="O56" s="8" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="24.95" customHeight="1">
       <c r="A57" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="O57" s="7" t="s">
-        <v>439</v>
+        <v>677</v>
+      </c>
+      <c r="O57" s="8" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="24.95" customHeight="1">
       <c r="A58" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="O58" s="7" t="s">
-        <v>440</v>
+        <v>678</v>
+      </c>
+      <c r="O58" s="8" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="24.95" customHeight="1">
       <c r="A59" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="O59" s="7" t="s">
-        <v>441</v>
+        <v>679</v>
+      </c>
+      <c r="O59" s="8" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="24.95" customHeight="1">
       <c r="A60" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="O60" s="6" t="s">
-        <v>442</v>
+        <v>680</v>
+      </c>
+      <c r="O60" s="8" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="24.95" customHeight="1">
       <c r="A61" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="O61" s="6" t="s">
-        <v>443</v>
+        <v>681</v>
+      </c>
+      <c r="O61" s="8" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A62" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="O62" s="6" t="s">
-        <v>444</v>
-      </c>
+      <c r="O62" s="6"/>
     </row>
     <row r="63" spans="1:15" ht="24.95" customHeight="1">
       <c r="A63" s="7" t="s">
-        <v>347</v>
+        <v>289</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>358</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="N63" s="7"/>
       <c r="O63" s="7" t="s">
-        <v>445</v>
+        <v>292</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A64" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="O64" s="7" t="s">
-        <v>446</v>
-      </c>
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="7"/>
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
+      <c r="N64" s="7"/>
+      <c r="O64" s="7"/>
     </row>
     <row r="65" spans="1:15" ht="24.95" customHeight="1">
       <c r="A65" s="7" t="s">
-        <v>349</v>
+        <v>606</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>360</v>
-      </c>
+        <v>687</v>
+      </c>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+      <c r="I65" s="7"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
+      <c r="N65" s="7"/>
       <c r="O65" s="7" t="s">
-        <v>447</v>
+        <v>690</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O66" s="6"/>
+      <c r="A66" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>688</v>
+      </c>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
+      <c r="I66" s="7"/>
+      <c r="J66" s="7"/>
+      <c r="K66" s="7"/>
+      <c r="L66" s="7"/>
+      <c r="M66" s="7"/>
+      <c r="N66" s="7"/>
+      <c r="O66" s="7" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="67" spans="1:15" ht="24.95" customHeight="1">
       <c r="A67" s="7" t="s">
-        <v>351</v>
-      </c>
+        <v>448</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="7"/>
+      <c r="L67" s="7"/>
+      <c r="M67" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="N67" s="7"/>
       <c r="O67" s="7" t="s">
-        <v>367</v>
+        <v>540</v>
       </c>
     </row>
     <row r="68" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A68" s="7" t="s">
-        <v>368</v>
+      <c r="A68" s="6" t="s">
+        <v>328</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>479</v>
+        <v>329</v>
       </c>
       <c r="O68" s="7" t="s">
-        <v>369</v>
+        <v>330</v>
       </c>
     </row>
     <row r="69" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A69" s="7" t="s">
-        <v>370</v>
+      <c r="A69" s="6" t="s">
+        <v>301</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>480</v>
+        <v>304</v>
       </c>
       <c r="O69" s="7" t="s">
-        <v>371</v>
+        <v>307</v>
       </c>
     </row>
     <row r="70" spans="1:15" ht="24.95" customHeight="1">
       <c r="A70" s="7" t="s">
-        <v>372</v>
+        <v>302</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>481</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+      <c r="I70" s="7"/>
+      <c r="J70" s="7"/>
+      <c r="K70" s="7"/>
+      <c r="L70" s="7"/>
+      <c r="M70" s="7"/>
+      <c r="N70" s="7"/>
       <c r="O70" s="7" t="s">
-        <v>373</v>
+        <v>308</v>
       </c>
     </row>
     <row r="71" spans="1:15" ht="24.95" customHeight="1">
       <c r="A71" s="7" t="s">
-        <v>374</v>
+        <v>303</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>483</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
+      <c r="N71" s="7"/>
       <c r="O71" s="7" t="s">
-        <v>375</v>
+        <v>309</v>
       </c>
     </row>
     <row r="72" spans="1:15" ht="24.95" customHeight="1">
       <c r="A72" s="7" t="s">
-        <v>376</v>
+        <v>310</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>482</v>
-      </c>
+        <v>311</v>
+      </c>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+      <c r="I72" s="7"/>
+      <c r="J72" s="7"/>
+      <c r="K72" s="7"/>
+      <c r="L72" s="7"/>
+      <c r="M72" s="7"/>
+      <c r="N72" s="7"/>
       <c r="O72" s="7" t="s">
-        <v>377</v>
+        <v>312</v>
       </c>
     </row>
     <row r="73" spans="1:15" ht="24.95" customHeight="1">
       <c r="A73" s="7" t="s">
-        <v>378</v>
+        <v>313</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>484</v>
-      </c>
-      <c r="O73" s="6" t="s">
-        <v>379</v>
+        <v>314</v>
+      </c>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
+      <c r="I73" s="7"/>
+      <c r="J73" s="7"/>
+      <c r="K73" s="7"/>
+      <c r="L73" s="7"/>
+      <c r="M73" s="7"/>
+      <c r="N73" s="7"/>
+      <c r="O73" s="7" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="74" spans="1:15" ht="24.95" customHeight="1">
       <c r="A74" s="7" t="s">
-        <v>380</v>
+        <v>318</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>485</v>
-      </c>
-      <c r="O74" s="6" t="s">
-        <v>381</v>
+        <v>315</v>
+      </c>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+      <c r="I74" s="7"/>
+      <c r="J74" s="7"/>
+      <c r="K74" s="7"/>
+      <c r="L74" s="7"/>
+      <c r="M74" s="7"/>
+      <c r="N74" s="7"/>
+      <c r="O74" s="7" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="75" spans="1:15" ht="24.95" customHeight="1">
       <c r="A75" s="7" t="s">
-        <v>382</v>
+        <v>319</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>586</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
+      <c r="I75" s="7"/>
+      <c r="J75" s="7"/>
+      <c r="K75" s="7"/>
+      <c r="L75" s="7"/>
+      <c r="M75" s="7"/>
+      <c r="N75" s="7"/>
       <c r="O75" s="7" t="s">
-        <v>383</v>
+        <v>323</v>
       </c>
     </row>
     <row r="76" spans="1:15" ht="24.95" customHeight="1">
       <c r="A76" s="7" t="s">
-        <v>384</v>
+        <v>326</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>487</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+      <c r="I76" s="7"/>
+      <c r="J76" s="7"/>
+      <c r="K76" s="7"/>
+      <c r="L76" s="7"/>
+      <c r="M76" s="7"/>
+      <c r="N76" s="7"/>
       <c r="O76" s="7" t="s">
-        <v>385</v>
+        <v>324</v>
       </c>
     </row>
     <row r="77" spans="1:15" ht="24.95" customHeight="1">
       <c r="A77" s="7" t="s">
-        <v>386</v>
+        <v>320</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>492</v>
-      </c>
+        <v>317</v>
+      </c>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
+      <c r="I77" s="7"/>
+      <c r="J77" s="7"/>
+      <c r="K77" s="7"/>
+      <c r="L77" s="7"/>
+      <c r="M77" s="7"/>
+      <c r="N77" s="7"/>
       <c r="O77" s="7" t="s">
-        <v>387</v>
+        <v>325</v>
       </c>
     </row>
     <row r="78" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A78" s="7" t="s">
-        <v>388</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>491</v>
-      </c>
-      <c r="O78" s="7" t="s">
-        <v>389</v>
-      </c>
+      <c r="O78" s="6"/>
     </row>
     <row r="79" spans="1:15" ht="24.95" customHeight="1">
       <c r="A79" s="7" t="s">
-        <v>390</v>
+        <v>339</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>488</v>
+        <v>334</v>
       </c>
       <c r="O79" s="7" t="s">
-        <v>391</v>
+        <v>333</v>
       </c>
     </row>
     <row r="80" spans="1:15" ht="24.95" customHeight="1">
       <c r="A80" s="7" t="s">
-        <v>392</v>
+        <v>335</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>489</v>
+        <v>337</v>
       </c>
       <c r="O80" s="7" t="s">
-        <v>393</v>
+        <v>336</v>
       </c>
     </row>
     <row r="81" spans="1:15" ht="24.95" customHeight="1">
       <c r="A81" s="7" t="s">
-        <v>394</v>
+        <v>338</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>490</v>
+        <v>350</v>
       </c>
       <c r="O81" s="7" t="s">
-        <v>395</v>
+        <v>340</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="24.95" customHeight="1">
       <c r="A82" s="7" t="s">
-        <v>396</v>
+        <v>341</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>486</v>
+        <v>352</v>
       </c>
       <c r="O82" s="7" t="s">
-        <v>397</v>
+        <v>439</v>
       </c>
     </row>
     <row r="83" spans="1:15" ht="24.95" customHeight="1">
       <c r="A83" s="7" t="s">
-        <v>398</v>
+        <v>342</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>353</v>
       </c>
       <c r="O83" s="7" t="s">
-        <v>399</v>
+        <v>440</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="24.95" customHeight="1">
       <c r="A84" s="7" t="s">
-        <v>587</v>
+        <v>343</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>588</v>
+        <v>354</v>
       </c>
       <c r="O84" s="7" t="s">
-        <v>589</v>
+        <v>441</v>
       </c>
     </row>
     <row r="85" spans="1:15" ht="24.95" customHeight="1">
       <c r="A85" s="7" t="s">
-        <v>400</v>
+        <v>344</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>493</v>
-      </c>
-      <c r="O85" s="7" t="s">
-        <v>401</v>
+        <v>355</v>
+      </c>
+      <c r="O85" s="6" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="86" spans="1:15" ht="24.95" customHeight="1">
       <c r="A86" s="7" t="s">
-        <v>402</v>
+        <v>345</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>494</v>
-      </c>
-      <c r="O86" s="7" t="s">
-        <v>403</v>
+        <v>356</v>
+      </c>
+      <c r="O86" s="6" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="87" spans="1:15" ht="24.95" customHeight="1">
       <c r="A87" s="7" t="s">
-        <v>593</v>
-      </c>
-      <c r="B87" s="7"/>
-      <c r="O87" s="7" t="s">
-        <v>594</v>
+        <v>346</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="O87" s="6" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="88" spans="1:15" ht="24.95" customHeight="1">
       <c r="A88" s="7" t="s">
-        <v>595</v>
-      </c>
-      <c r="B88" s="7"/>
+        <v>347</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>358</v>
+      </c>
       <c r="O88" s="7" t="s">
-        <v>602</v>
+        <v>445</v>
       </c>
     </row>
     <row r="89" spans="1:15" ht="24.95" customHeight="1">
       <c r="A89" s="7" t="s">
-        <v>596</v>
-      </c>
-      <c r="B89" s="7"/>
+        <v>348</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>359</v>
+      </c>
       <c r="O89" s="7" t="s">
-        <v>603</v>
+        <v>446</v>
       </c>
     </row>
     <row r="90" spans="1:15" ht="24.95" customHeight="1">
       <c r="A90" s="7" t="s">
-        <v>597</v>
-      </c>
-      <c r="B90" s="7"/>
+        <v>349</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>360</v>
+      </c>
       <c r="O90" s="7" t="s">
-        <v>604</v>
+        <v>447</v>
       </c>
     </row>
     <row r="91" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A91" s="7" t="s">
-        <v>598</v>
-      </c>
-      <c r="B91" s="7"/>
-      <c r="O91" s="7" t="s">
-        <v>605</v>
-      </c>
+      <c r="O91" s="6"/>
     </row>
     <row r="92" spans="1:15" ht="24.95" customHeight="1">
       <c r="A92" s="7" t="s">
-        <v>599</v>
-      </c>
-      <c r="B92" s="7"/>
+        <v>351</v>
+      </c>
       <c r="O92" s="7" t="s">
-        <v>606</v>
+        <v>367</v>
       </c>
     </row>
     <row r="93" spans="1:15" ht="24.95" customHeight="1">
       <c r="A93" s="7" t="s">
-        <v>600</v>
-      </c>
-      <c r="B93" s="7"/>
+        <v>368</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>477</v>
+      </c>
       <c r="O93" s="7" t="s">
-        <v>607</v>
+        <v>369</v>
       </c>
     </row>
     <row r="94" spans="1:15" ht="24.95" customHeight="1">
       <c r="A94" s="7" t="s">
-        <v>601</v>
-      </c>
-      <c r="B94" s="7"/>
+        <v>370</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>478</v>
+      </c>
       <c r="O94" s="7" t="s">
-        <v>608</v>
+        <v>371</v>
       </c>
     </row>
     <row r="95" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A95" s="7"/>
-      <c r="B95" s="7"/>
-      <c r="O95" s="7"/>
+      <c r="A95" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="O95" s="7" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="96" spans="1:15" ht="24.95" customHeight="1">
       <c r="A96" s="7" t="s">
-        <v>404</v>
+        <v>374</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>405</v>
+        <v>481</v>
       </c>
       <c r="O96" s="7" t="s">
-        <v>405</v>
+        <v>375</v>
       </c>
     </row>
     <row r="97" spans="1:15" ht="24.95" customHeight="1">
       <c r="A97" s="7" t="s">
-        <v>406</v>
+        <v>376</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>590</v>
+        <v>480</v>
       </c>
       <c r="O97" s="7" t="s">
-        <v>407</v>
+        <v>377</v>
       </c>
     </row>
     <row r="98" spans="1:15" ht="24.95" customHeight="1">
       <c r="A98" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>409</v>
-      </c>
-      <c r="O98" s="7" t="s">
-        <v>410</v>
+        <v>378</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="O98" s="6" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="99" spans="1:15" ht="24.95" customHeight="1">
       <c r="A99" s="7" t="s">
-        <v>411</v>
+        <v>380</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>457</v>
-      </c>
-      <c r="O99" s="7" t="s">
-        <v>412</v>
+        <v>483</v>
+      </c>
+      <c r="O99" s="6" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="100" spans="1:15" ht="24.95" customHeight="1">
       <c r="A100" s="7" t="s">
-        <v>413</v>
+        <v>382</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>591</v>
+        <v>582</v>
       </c>
       <c r="O100" s="7" t="s">
-        <v>414</v>
+        <v>383</v>
       </c>
     </row>
     <row r="101" spans="1:15" ht="24.95" customHeight="1">
       <c r="A101" s="7" t="s">
-        <v>415</v>
+        <v>384</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>458</v>
+        <v>485</v>
       </c>
       <c r="O101" s="7" t="s">
-        <v>416</v>
+        <v>385</v>
       </c>
     </row>
     <row r="102" spans="1:15" ht="24.95" customHeight="1">
       <c r="A102" s="7" t="s">
-        <v>417</v>
+        <v>386</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>459</v>
+        <v>490</v>
       </c>
       <c r="O102" s="7" t="s">
-        <v>418</v>
+        <v>387</v>
       </c>
     </row>
     <row r="103" spans="1:15" ht="24.95" customHeight="1">
       <c r="A103" s="7" t="s">
-        <v>419</v>
+        <v>388</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>460</v>
+        <v>489</v>
       </c>
       <c r="O103" s="7" t="s">
-        <v>420</v>
+        <v>389</v>
       </c>
     </row>
     <row r="104" spans="1:15" ht="24.95" customHeight="1">
       <c r="A104" s="7" t="s">
-        <v>421</v>
+        <v>390</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>422</v>
+        <v>486</v>
       </c>
       <c r="O104" s="7" t="s">
-        <v>422</v>
+        <v>391</v>
       </c>
     </row>
     <row r="105" spans="1:15" ht="24.95" customHeight="1">
       <c r="A105" s="7" t="s">
-        <v>423</v>
+        <v>392</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>487</v>
       </c>
       <c r="O105" s="7" t="s">
-        <v>424</v>
+        <v>393</v>
       </c>
     </row>
     <row r="106" spans="1:15" ht="24.95" customHeight="1">
       <c r="A106" s="7" t="s">
-        <v>592</v>
+        <v>394</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>488</v>
       </c>
       <c r="O106" s="7" t="s">
-        <v>425</v>
+        <v>395</v>
       </c>
     </row>
     <row r="107" spans="1:15" ht="24.95" customHeight="1">
       <c r="A107" s="7" t="s">
-        <v>426</v>
+        <v>396</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>484</v>
       </c>
       <c r="O107" s="7" t="s">
-        <v>427</v>
+        <v>397</v>
       </c>
     </row>
     <row r="108" spans="1:15" ht="24.95" customHeight="1">
       <c r="A108" s="7" t="s">
-        <v>428</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>429</v>
+        <v>398</v>
       </c>
       <c r="O108" s="7" t="s">
-        <v>430</v>
+        <v>399</v>
       </c>
     </row>
     <row r="109" spans="1:15" ht="24.95" customHeight="1">
       <c r="A109" s="7" t="s">
-        <v>432</v>
+        <v>583</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>584</v>
       </c>
       <c r="O109" s="7" t="s">
-        <v>431</v>
+        <v>585</v>
       </c>
     </row>
     <row r="110" spans="1:15" ht="24.95" customHeight="1">
       <c r="A110" s="7" t="s">
-        <v>433</v>
+        <v>400</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>456</v>
+        <v>491</v>
       </c>
       <c r="O110" s="7" t="s">
-        <v>434</v>
+        <v>401</v>
       </c>
     </row>
     <row r="111" spans="1:15" ht="24.95" customHeight="1">
       <c r="A111" s="7" t="s">
-        <v>435</v>
+        <v>402</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>455</v>
+        <v>492</v>
       </c>
       <c r="O111" s="7" t="s">
-        <v>436</v>
+        <v>403</v>
       </c>
     </row>
     <row r="112" spans="1:15" ht="24.95" customHeight="1">
       <c r="A112" s="7" t="s">
-        <v>453</v>
-      </c>
-      <c r="B112" s="7" t="s">
-        <v>451</v>
-      </c>
+        <v>589</v>
+      </c>
+      <c r="B112" s="7"/>
       <c r="O112" s="7" t="s">
-        <v>437</v>
+        <v>590</v>
       </c>
     </row>
     <row r="113" spans="1:15" ht="24.95" customHeight="1">
       <c r="A113" s="7" t="s">
-        <v>454</v>
-      </c>
-      <c r="B113" s="6" t="s">
-        <v>452</v>
-      </c>
+        <v>591</v>
+      </c>
+      <c r="B113" s="7"/>
       <c r="O113" s="7" t="s">
-        <v>438</v>
+        <v>598</v>
       </c>
     </row>
     <row r="114" spans="1:15" ht="24.95" customHeight="1">
       <c r="A114" s="7" t="s">
-        <v>461</v>
-      </c>
-      <c r="B114" s="7" t="s">
-        <v>473</v>
-      </c>
-      <c r="O114" s="8" t="s">
-        <v>467</v>
+        <v>592</v>
+      </c>
+      <c r="B114" s="7"/>
+      <c r="O114" s="7" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="115" spans="1:15" ht="24.95" customHeight="1">
       <c r="A115" s="7" t="s">
-        <v>462</v>
-      </c>
-      <c r="B115" s="7" t="s">
-        <v>474</v>
-      </c>
+        <v>593</v>
+      </c>
+      <c r="B115" s="7"/>
       <c r="O115" s="7" t="s">
-        <v>468</v>
+        <v>600</v>
       </c>
     </row>
     <row r="116" spans="1:15" ht="24.95" customHeight="1">
       <c r="A116" s="7" t="s">
-        <v>463</v>
-      </c>
-      <c r="B116" s="7" t="s">
-        <v>475</v>
-      </c>
+        <v>594</v>
+      </c>
+      <c r="B116" s="7"/>
       <c r="O116" s="7" t="s">
-        <v>469</v>
+        <v>601</v>
       </c>
     </row>
     <row r="117" spans="1:15" ht="24.95" customHeight="1">
       <c r="A117" s="7" t="s">
-        <v>464</v>
-      </c>
-      <c r="B117" s="7" t="s">
-        <v>476</v>
-      </c>
+        <v>595</v>
+      </c>
+      <c r="B117" s="7"/>
       <c r="O117" s="7" t="s">
-        <v>470</v>
+        <v>602</v>
       </c>
     </row>
     <row r="118" spans="1:15" ht="24.95" customHeight="1">
       <c r="A118" s="7" t="s">
-        <v>465</v>
-      </c>
-      <c r="B118" s="7" t="s">
-        <v>478</v>
-      </c>
+        <v>596</v>
+      </c>
+      <c r="B118" s="7"/>
       <c r="O118" s="7" t="s">
-        <v>471</v>
+        <v>603</v>
       </c>
     </row>
     <row r="119" spans="1:15" ht="24.95" customHeight="1">
       <c r="A119" s="7" t="s">
-        <v>466</v>
-      </c>
-      <c r="B119" s="7" t="s">
-        <v>477</v>
-      </c>
+        <v>597</v>
+      </c>
+      <c r="B119" s="7"/>
       <c r="O119" s="7" t="s">
-        <v>472</v>
+        <v>604</v>
       </c>
     </row>
     <row r="120" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A120" s="7" t="s">
-        <v>495</v>
-      </c>
-      <c r="B120" s="7" t="s">
-        <v>499</v>
-      </c>
-      <c r="O120" s="7" t="s">
-        <v>498</v>
-      </c>
+      <c r="A120" s="7"/>
+      <c r="B120" s="7"/>
+      <c r="O120" s="7"/>
     </row>
     <row r="121" spans="1:15" ht="24.95" customHeight="1">
       <c r="A121" s="7" t="s">
-        <v>496</v>
+        <v>404</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>500</v>
+        <v>405</v>
       </c>
       <c r="O121" s="7" t="s">
-        <v>497</v>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A122" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>586</v>
+      </c>
+      <c r="O122" s="7" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="123" spans="1:15" ht="24.95" customHeight="1">
       <c r="A123" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="B123" s="7" t="s">
-        <v>362</v>
+        <v>408</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>409</v>
       </c>
       <c r="O123" s="7" t="s">
-        <v>365</v>
+        <v>410</v>
       </c>
     </row>
     <row r="124" spans="1:15" ht="24.95" customHeight="1">
       <c r="A124" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="B124" s="6" t="s">
-        <v>364</v>
+        <v>411</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>455</v>
       </c>
       <c r="O124" s="7" t="s">
-        <v>366</v>
+        <v>412</v>
       </c>
     </row>
     <row r="125" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A125" s="6" t="s">
-        <v>501</v>
+      <c r="A125" s="7" t="s">
+        <v>413</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>508</v>
+        <v>587</v>
       </c>
       <c r="O125" s="7" t="s">
-        <v>524</v>
+        <v>414</v>
       </c>
     </row>
     <row r="126" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A126" s="6" t="s">
-        <v>502</v>
+      <c r="A126" s="7" t="s">
+        <v>415</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>509</v>
+        <v>456</v>
       </c>
       <c r="O126" s="7" t="s">
-        <v>525</v>
+        <v>416</v>
       </c>
     </row>
     <row r="127" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A127" s="6" t="s">
-        <v>503</v>
+      <c r="A127" s="7" t="s">
+        <v>417</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>510</v>
-      </c>
-      <c r="O127" s="10" t="s">
-        <v>526</v>
+        <v>457</v>
+      </c>
+      <c r="O127" s="7" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="128" spans="1:15" ht="24.95" customHeight="1">
       <c r="A128" s="7" t="s">
-        <v>504</v>
+        <v>419</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>511</v>
+        <v>458</v>
       </c>
       <c r="O128" s="7" t="s">
-        <v>527</v>
+        <v>420</v>
       </c>
     </row>
     <row r="129" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A129" s="6" t="s">
-        <v>505</v>
+      <c r="A129" s="7" t="s">
+        <v>421</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>512</v>
+        <v>422</v>
       </c>
       <c r="O129" s="7" t="s">
-        <v>528</v>
+        <v>422</v>
       </c>
     </row>
     <row r="130" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A130" s="6" t="s">
-        <v>506</v>
-      </c>
-      <c r="B130" s="7" t="s">
-        <v>513</v>
-      </c>
-      <c r="O130" s="10" t="s">
-        <v>529</v>
+      <c r="A130" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="O130" s="7" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="131" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A131" s="6" t="s">
-        <v>507</v>
-      </c>
-      <c r="B131" s="7" t="s">
-        <v>514</v>
-      </c>
-      <c r="O131" s="10" t="s">
-        <v>530</v>
+      <c r="A131" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="O131" s="7" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="132" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O132" s="10"/>
+      <c r="A132" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="O132" s="7" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="133" spans="1:15" ht="24.95" customHeight="1">
       <c r="A133" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="B133" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="O133" s="10" t="s">
-        <v>517</v>
+        <v>428</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="O133" s="7" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="134" spans="1:15" ht="24.95" customHeight="1">
       <c r="A134" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="O134" s="7" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A135" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="O135" s="7" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A136" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="O136" s="7" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A137" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="O137" s="7" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A138" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="O138" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A139" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="O139" s="8" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A140" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="O140" s="7" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A141" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="O141" s="7" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A142" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="O142" s="7" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A143" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="O143" s="7" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A144" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="O144" s="7" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A145" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="O145" s="7" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A146" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="B146" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="O146" s="7" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A148" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="B148" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="O148" s="7" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A149" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="O149" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A150" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="O150" s="7" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A151" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="O151" s="7" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A152" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="O152" s="10" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A153" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>509</v>
+      </c>
+      <c r="O153" s="7" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A154" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="B154" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="O154" s="7" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A155" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="B155" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="O155" s="10" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A156" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="O156" s="10" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" ht="24.95" customHeight="1">
+      <c r="O157" s="10"/>
+    </row>
+    <row r="158" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A158" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="B158" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="O158" s="10" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A159" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="B159" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="O159" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="B134" s="7" t="s">
-        <v>520</v>
-      </c>
-      <c r="O134" s="10" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="135" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O135" s="10"/>
-    </row>
-    <row r="136" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O136" s="10"/>
-    </row>
-    <row r="137" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O137" s="10"/>
-    </row>
-    <row r="138" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O138" s="6"/>
-    </row>
-    <row r="139" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O139" s="6"/>
-    </row>
-    <row r="140" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O140" s="6"/>
-    </row>
-    <row r="141" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O141" s="6"/>
-    </row>
-    <row r="142" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O142" s="6"/>
-    </row>
-    <row r="143" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O143" s="6"/>
-    </row>
-    <row r="144" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O144" s="6"/>
-    </row>
-    <row r="145" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O145" s="6"/>
-    </row>
-    <row r="146" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O146" s="6"/>
-    </row>
-    <row r="147" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O147" s="10"/>
-    </row>
-    <row r="148" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O148" s="10"/>
-    </row>
-    <row r="149" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O149" s="10"/>
-    </row>
-    <row r="150" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O150" s="6"/>
-    </row>
-    <row r="151" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O151" s="10"/>
-    </row>
-    <row r="153" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O153" s="10"/>
-    </row>
-    <row r="154" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O154" s="6"/>
-    </row>
-    <row r="155" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O155" s="6"/>
-    </row>
-    <row r="156" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O156" s="10"/>
-    </row>
-    <row r="157" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O157" s="10"/>
-    </row>
-    <row r="158" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O158" s="6"/>
-    </row>
-    <row r="159" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O159" s="10"/>
-    </row>
-    <row r="160" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O160" s="6"/>
-    </row>
-    <row r="161" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O161" s="6"/>
-    </row>
-    <row r="162" spans="1:15" ht="24.95" customHeight="1">
+    </row>
+    <row r="160" spans="1:15" ht="24.95" customHeight="1">
+      <c r="O160" s="10"/>
+    </row>
+    <row r="161" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O161" s="10"/>
+    </row>
+    <row r="162" spans="15:15" ht="24.95" customHeight="1">
       <c r="O162" s="10"/>
     </row>
-    <row r="163" spans="1:15" ht="24.95" customHeight="1">
+    <row r="163" spans="15:15" ht="24.95" customHeight="1">
       <c r="O163" s="6"/>
     </row>
-    <row r="164" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O164" s="10"/>
-    </row>
-    <row r="165" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A165" s="7" t="s">
+    <row r="164" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O164" s="6"/>
+    </row>
+    <row r="165" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O165" s="6"/>
+    </row>
+    <row r="166" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O166" s="6"/>
+    </row>
+    <row r="167" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O167" s="6"/>
+    </row>
+    <row r="168" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O168" s="6"/>
+    </row>
+    <row r="169" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O169" s="6"/>
+    </row>
+    <row r="170" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O170" s="6"/>
+    </row>
+    <row r="171" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O171" s="6"/>
+    </row>
+    <row r="172" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O172" s="10"/>
+    </row>
+    <row r="173" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O173" s="10"/>
+    </row>
+    <row r="174" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O174" s="10"/>
+    </row>
+    <row r="175" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O175" s="6"/>
+    </row>
+    <row r="176" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O176" s="10"/>
+    </row>
+    <row r="178" spans="1:15" ht="24.95" customHeight="1">
+      <c r="O178" s="10"/>
+    </row>
+    <row r="179" spans="1:15" ht="24.95" customHeight="1">
+      <c r="O179" s="6"/>
+    </row>
+    <row r="180" spans="1:15" ht="24.95" customHeight="1">
+      <c r="O180" s="6"/>
+    </row>
+    <row r="181" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A181" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="O181" s="8" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A182" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B182" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="O182" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="183" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A183" s="7"/>
+      <c r="B183" s="7"/>
+      <c r="C183" s="7"/>
+      <c r="D183" s="7"/>
+      <c r="E183" s="7"/>
+      <c r="F183" s="7"/>
+      <c r="G183" s="7"/>
+      <c r="H183" s="7"/>
+      <c r="I183" s="7"/>
+      <c r="J183" s="7"/>
+      <c r="K183" s="7"/>
+      <c r="L183" s="7"/>
+      <c r="M183" s="7"/>
+      <c r="N183" s="7"/>
+      <c r="O183" s="7"/>
+    </row>
+    <row r="184" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A184" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="B184" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="C184" s="7"/>
+      <c r="D184" s="7"/>
+      <c r="E184" s="7"/>
+      <c r="F184" s="7"/>
+      <c r="G184" s="7"/>
+      <c r="H184" s="7"/>
+      <c r="I184" s="7"/>
+      <c r="J184" s="7"/>
+      <c r="K184" s="7"/>
+      <c r="L184" s="7"/>
+      <c r="M184" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="N184" s="7"/>
+      <c r="O184" s="7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="185" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A185" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="B185" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C185" s="7"/>
+      <c r="D185" s="7"/>
+      <c r="E185" s="7"/>
+      <c r="F185" s="7"/>
+      <c r="G185" s="7"/>
+      <c r="H185" s="7"/>
+      <c r="I185" s="7"/>
+      <c r="J185" s="7"/>
+      <c r="K185" s="7"/>
+      <c r="L185" s="7"/>
+      <c r="M185" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="N185" s="7"/>
+      <c r="O185" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="186" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A186" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="B186" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C186" s="7"/>
+      <c r="D186" s="7"/>
+      <c r="E186" s="7"/>
+      <c r="F186" s="7"/>
+      <c r="G186" s="7"/>
+      <c r="H186" s="7"/>
+      <c r="I186" s="7"/>
+      <c r="J186" s="7"/>
+      <c r="K186" s="7"/>
+      <c r="L186" s="7"/>
+      <c r="M186" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="N186" s="7"/>
+      <c r="O186" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="187" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A187" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B187" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="C187" s="7"/>
+      <c r="D187" s="7"/>
+      <c r="E187" s="7"/>
+      <c r="F187" s="7"/>
+      <c r="G187" s="7"/>
+      <c r="H187" s="7"/>
+      <c r="I187" s="7"/>
+      <c r="J187" s="7"/>
+      <c r="K187" s="7"/>
+      <c r="L187" s="7"/>
+      <c r="M187" s="7"/>
+      <c r="N187" s="7"/>
+      <c r="O187" s="7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="188" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A188" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="B188" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="C188" s="7"/>
+      <c r="D188" s="7"/>
+      <c r="E188" s="7"/>
+      <c r="F188" s="7"/>
+      <c r="G188" s="7"/>
+      <c r="H188" s="7"/>
+      <c r="I188" s="7"/>
+      <c r="J188" s="7"/>
+      <c r="K188" s="7"/>
+      <c r="L188" s="7"/>
+      <c r="M188" s="7"/>
+      <c r="N188" s="7"/>
+      <c r="O188" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A189" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="B189" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="C189" s="7"/>
+      <c r="D189" s="7"/>
+      <c r="E189" s="7"/>
+      <c r="F189" s="7"/>
+      <c r="G189" s="7"/>
+      <c r="H189" s="7"/>
+      <c r="I189" s="7"/>
+      <c r="J189" s="7"/>
+      <c r="K189" s="7"/>
+      <c r="L189" s="7"/>
+      <c r="M189" s="7"/>
+      <c r="N189" s="7"/>
+      <c r="O189" s="7" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="190" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A190" s="7"/>
+      <c r="B190" s="7"/>
+      <c r="C190" s="7"/>
+      <c r="D190" s="7"/>
+      <c r="E190" s="7"/>
+      <c r="F190" s="7"/>
+      <c r="G190" s="7"/>
+      <c r="H190" s="7"/>
+      <c r="I190" s="7"/>
+      <c r="J190" s="7"/>
+      <c r="K190" s="7"/>
+      <c r="L190" s="7"/>
+      <c r="M190" s="7"/>
+      <c r="N190" s="7"/>
+      <c r="O190" s="7"/>
+    </row>
+    <row r="191" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A191" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="B165" s="7" t="s">
+      <c r="B191" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="O165" s="7" t="s">
+      <c r="O191" s="7" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="166" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O166" s="10"/>
-    </row>
-    <row r="167" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O167" s="10"/>
-    </row>
-    <row r="168" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O168" s="6"/>
-    </row>
-    <row r="169" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O169" s="6"/>
-    </row>
-    <row r="170" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O170" s="6"/>
-    </row>
-    <row r="171" spans="1:15" ht="24.95" customHeight="1">
-      <c r="B171" s="9"/>
-      <c r="M171" s="9"/>
-    </row>
-    <row r="172" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O172" s="6"/>
-    </row>
-    <row r="173" spans="1:15" ht="24.95" customHeight="1">
-      <c r="B173" s="9"/>
-      <c r="M173" s="9"/>
-    </row>
-    <row r="174" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O174" s="6"/>
-    </row>
-    <row r="175" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O175" s="6"/>
-    </row>
-    <row r="176" spans="1:15" ht="24.95" customHeight="1">
-      <c r="O176" s="6"/>
-    </row>
-    <row r="177" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O177" s="6"/>
-    </row>
-    <row r="178" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O178" s="6"/>
-    </row>
-    <row r="179" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O179" s="6"/>
-    </row>
-    <row r="180" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O180" s="6"/>
-    </row>
-    <row r="181" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O181" s="6"/>
-    </row>
-    <row r="182" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O182" s="6"/>
-    </row>
-    <row r="183" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O183" s="6"/>
-    </row>
-    <row r="184" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O184" s="6"/>
-    </row>
-    <row r="185" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O185" s="6"/>
-    </row>
-    <row r="186" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O186" s="6"/>
-    </row>
-    <row r="187" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O187" s="6"/>
-    </row>
-    <row r="188" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O188" s="6"/>
-    </row>
-    <row r="189" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O189" s="6"/>
-    </row>
-    <row r="190" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O190" s="6"/>
-    </row>
-    <row r="191" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O191" s="6"/>
-    </row>
-    <row r="192" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O192" s="6"/>
-    </row>
-    <row r="193" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O193" s="6"/>
-    </row>
-    <row r="194" spans="15:15" ht="24.95" customHeight="1">
+    <row r="192" spans="1:15" ht="24.95" customHeight="1">
+      <c r="O192" s="10"/>
+    </row>
+    <row r="193" spans="2:15" ht="24.95" customHeight="1">
+      <c r="O193" s="10"/>
+    </row>
+    <row r="194" spans="2:15" ht="24.95" customHeight="1">
       <c r="O194" s="6"/>
     </row>
-    <row r="195" spans="15:15" ht="24.95" customHeight="1">
+    <row r="195" spans="2:15" ht="24.95" customHeight="1">
       <c r="O195" s="6"/>
     </row>
-    <row r="196" spans="15:15" ht="24.95" customHeight="1">
+    <row r="196" spans="2:15" ht="24.95" customHeight="1">
       <c r="O196" s="6"/>
     </row>
-    <row r="197" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O197" s="6"/>
-    </row>
-    <row r="198" spans="15:15" ht="24.95" customHeight="1">
+    <row r="197" spans="2:15" ht="24.95" customHeight="1">
+      <c r="B197" s="9"/>
+      <c r="M197" s="9"/>
+    </row>
+    <row r="198" spans="2:15" ht="24.95" customHeight="1">
       <c r="O198" s="6"/>
     </row>
-    <row r="199" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O199" s="6"/>
-    </row>
-    <row r="200" spans="15:15" ht="24.95" customHeight="1">
+    <row r="199" spans="2:15" ht="24.95" customHeight="1">
+      <c r="B199" s="9"/>
+      <c r="M199" s="9"/>
+    </row>
+    <row r="200" spans="2:15" ht="24.95" customHeight="1">
       <c r="O200" s="6"/>
     </row>
-    <row r="201" spans="15:15" ht="24.95" customHeight="1">
+    <row r="201" spans="2:15" ht="24.95" customHeight="1">
       <c r="O201" s="6"/>
     </row>
-    <row r="202" spans="15:15" ht="24.95" customHeight="1">
+    <row r="202" spans="2:15" ht="24.95" customHeight="1">
       <c r="O202" s="6"/>
     </row>
-    <row r="203" spans="15:15" ht="24.95" customHeight="1">
+    <row r="203" spans="2:15" ht="24.95" customHeight="1">
       <c r="O203" s="6"/>
     </row>
-    <row r="204" spans="15:15" ht="24.95" customHeight="1">
+    <row r="204" spans="2:15" ht="24.95" customHeight="1">
       <c r="O204" s="6"/>
     </row>
-    <row r="205" spans="15:15" ht="24.95" customHeight="1">
+    <row r="205" spans="2:15" ht="24.95" customHeight="1">
       <c r="O205" s="6"/>
     </row>
-    <row r="206" spans="15:15" ht="24.95" customHeight="1">
+    <row r="206" spans="2:15" ht="24.95" customHeight="1">
       <c r="O206" s="6"/>
     </row>
-    <row r="207" spans="15:15" ht="24.95" customHeight="1">
+    <row r="207" spans="2:15" ht="24.95" customHeight="1">
       <c r="O207" s="6"/>
     </row>
-    <row r="208" spans="15:15" ht="24.95" customHeight="1">
+    <row r="208" spans="2:15" ht="24.95" customHeight="1">
       <c r="O208" s="6"/>
     </row>
     <row r="209" spans="15:15" ht="24.95" customHeight="1">
@@ -5761,6 +6308,9 @@
     <row r="514" spans="15:15" ht="24.95" customHeight="1">
       <c r="O514" s="6"/>
     </row>
+    <row r="515" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O515" s="6"/>
+    </row>
     <row r="516" spans="15:15" ht="24.95" customHeight="1">
       <c r="O516" s="6"/>
     </row>
@@ -5836,9 +6386,6 @@
     <row r="540" spans="15:15" ht="24.95" customHeight="1">
       <c r="O540" s="6"/>
     </row>
-    <row r="541" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O541" s="6"/>
-    </row>
     <row r="542" spans="15:15" ht="24.95" customHeight="1">
       <c r="O542" s="6"/>
     </row>
@@ -6904,65 +7451,52 @@
     <row r="896" spans="15:15" ht="24.95" customHeight="1">
       <c r="O896" s="6"/>
     </row>
-    <row r="897" spans="1:15" ht="24.95" customHeight="1">
+    <row r="897" spans="15:15" ht="24.95" customHeight="1">
       <c r="O897" s="6"/>
     </row>
-    <row r="898" spans="1:15" ht="24.95" customHeight="1">
+    <row r="898" spans="15:15" ht="24.95" customHeight="1">
       <c r="O898" s="6"/>
     </row>
-    <row r="899" spans="1:15" ht="24.95" customHeight="1">
+    <row r="899" spans="15:15" ht="24.95" customHeight="1">
       <c r="O899" s="6"/>
     </row>
-    <row r="900" spans="1:15" ht="24.95" customHeight="1">
+    <row r="900" spans="15:15" ht="24.95" customHeight="1">
       <c r="O900" s="6"/>
     </row>
-    <row r="901" spans="1:15" ht="24.95" customHeight="1">
+    <row r="901" spans="15:15" ht="24.95" customHeight="1">
       <c r="O901" s="6"/>
     </row>
-    <row r="902" spans="1:15" ht="24.95" customHeight="1">
+    <row r="902" spans="15:15" ht="24.95" customHeight="1">
       <c r="O902" s="6"/>
     </row>
-    <row r="903" spans="1:15" ht="24.95" customHeight="1">
+    <row r="903" spans="15:15" ht="24.95" customHeight="1">
       <c r="O903" s="6"/>
     </row>
-    <row r="904" spans="1:15" ht="24.95" customHeight="1">
+    <row r="904" spans="15:15" ht="24.95" customHeight="1">
       <c r="O904" s="6"/>
     </row>
-    <row r="905" spans="1:15" ht="24.95" customHeight="1">
+    <row r="905" spans="15:15" ht="24.95" customHeight="1">
       <c r="O905" s="6"/>
     </row>
-    <row r="906" spans="1:15" ht="24.95" customHeight="1">
+    <row r="906" spans="15:15" ht="24.95" customHeight="1">
       <c r="O906" s="6"/>
     </row>
-    <row r="907" spans="1:15" ht="24.95" customHeight="1">
+    <row r="907" spans="15:15" ht="24.95" customHeight="1">
       <c r="O907" s="6"/>
     </row>
-    <row r="908" spans="1:15" ht="24.95" customHeight="1">
+    <row r="908" spans="15:15" ht="24.95" customHeight="1">
       <c r="O908" s="6"/>
     </row>
-    <row r="909" spans="1:15" ht="24.95" customHeight="1">
-      <c r="A909" s="11"/>
-      <c r="B909" s="11"/>
-      <c r="D909" s="11"/>
-      <c r="E909" s="11"/>
-      <c r="F909" s="11"/>
-      <c r="G909" s="11"/>
-      <c r="H909" s="11"/>
-      <c r="I909" s="11"/>
-      <c r="J909" s="11"/>
-      <c r="K909" s="11"/>
-      <c r="L909" s="11"/>
-      <c r="M909" s="11"/>
-      <c r="N909" s="11"/>
-      <c r="O909" s="12"/>
-    </row>
-    <row r="910" spans="1:15" ht="24.95" customHeight="1">
+    <row r="909" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O909" s="6"/>
+    </row>
+    <row r="910" spans="15:15" ht="24.95" customHeight="1">
       <c r="O910" s="6"/>
     </row>
-    <row r="911" spans="1:15" ht="24.95" customHeight="1">
+    <row r="911" spans="15:15" ht="24.95" customHeight="1">
       <c r="O911" s="6"/>
     </row>
-    <row r="912" spans="1:15" ht="24.95" customHeight="1">
+    <row r="912" spans="15:15" ht="24.95" customHeight="1">
       <c r="O912" s="6"/>
     </row>
     <row r="913" spans="15:15" ht="24.95" customHeight="1">
@@ -7013,52 +7547,65 @@
     <row r="928" spans="15:15" ht="24.95" customHeight="1">
       <c r="O928" s="6"/>
     </row>
-    <row r="929" spans="15:15" ht="24.95" customHeight="1">
+    <row r="929" spans="1:15" ht="24.95" customHeight="1">
       <c r="O929" s="6"/>
     </row>
-    <row r="930" spans="15:15" ht="24.95" customHeight="1">
+    <row r="930" spans="1:15" ht="24.95" customHeight="1">
       <c r="O930" s="6"/>
     </row>
-    <row r="931" spans="15:15" ht="24.95" customHeight="1">
+    <row r="931" spans="1:15" ht="24.95" customHeight="1">
       <c r="O931" s="6"/>
     </row>
-    <row r="932" spans="15:15" ht="24.95" customHeight="1">
+    <row r="932" spans="1:15" ht="24.95" customHeight="1">
       <c r="O932" s="6"/>
     </row>
-    <row r="933" spans="15:15" ht="24.95" customHeight="1">
+    <row r="933" spans="1:15" ht="24.95" customHeight="1">
       <c r="O933" s="6"/>
     </row>
-    <row r="934" spans="15:15" ht="24.95" customHeight="1">
+    <row r="934" spans="1:15" ht="24.95" customHeight="1">
       <c r="O934" s="6"/>
     </row>
-    <row r="935" spans="15:15" ht="24.95" customHeight="1">
-      <c r="O935" s="6"/>
-    </row>
-    <row r="936" spans="15:15" ht="24.95" customHeight="1">
+    <row r="935" spans="1:15" ht="24.95" customHeight="1">
+      <c r="A935" s="11"/>
+      <c r="B935" s="11"/>
+      <c r="D935" s="11"/>
+      <c r="E935" s="11"/>
+      <c r="F935" s="11"/>
+      <c r="G935" s="11"/>
+      <c r="H935" s="11"/>
+      <c r="I935" s="11"/>
+      <c r="J935" s="11"/>
+      <c r="K935" s="11"/>
+      <c r="L935" s="11"/>
+      <c r="M935" s="11"/>
+      <c r="N935" s="11"/>
+      <c r="O935" s="12"/>
+    </row>
+    <row r="936" spans="1:15" ht="24.95" customHeight="1">
       <c r="O936" s="6"/>
     </row>
-    <row r="937" spans="15:15" ht="24.95" customHeight="1">
+    <row r="937" spans="1:15" ht="24.95" customHeight="1">
       <c r="O937" s="6"/>
     </row>
-    <row r="938" spans="15:15" ht="24.95" customHeight="1">
+    <row r="938" spans="1:15" ht="24.95" customHeight="1">
       <c r="O938" s="6"/>
     </row>
-    <row r="939" spans="15:15" ht="24.95" customHeight="1">
+    <row r="939" spans="1:15" ht="24.95" customHeight="1">
       <c r="O939" s="6"/>
     </row>
-    <row r="940" spans="15:15" ht="24.95" customHeight="1">
+    <row r="940" spans="1:15" ht="24.95" customHeight="1">
       <c r="O940" s="6"/>
     </row>
-    <row r="941" spans="15:15" ht="24.95" customHeight="1">
+    <row r="941" spans="1:15" ht="24.95" customHeight="1">
       <c r="O941" s="6"/>
     </row>
-    <row r="942" spans="15:15" ht="24.95" customHeight="1">
+    <row r="942" spans="1:15" ht="24.95" customHeight="1">
       <c r="O942" s="6"/>
     </row>
-    <row r="943" spans="15:15" ht="24.95" customHeight="1">
+    <row r="943" spans="1:15" ht="24.95" customHeight="1">
       <c r="O943" s="6"/>
     </row>
-    <row r="944" spans="15:15" ht="24.95" customHeight="1">
+    <row r="944" spans="1:15" ht="24.95" customHeight="1">
       <c r="O944" s="6"/>
     </row>
     <row r="945" spans="15:15" ht="24.95" customHeight="1">
@@ -8471,8 +9018,86 @@
     <row r="1414" spans="15:15" ht="24.95" customHeight="1">
       <c r="O1414" s="6"/>
     </row>
+    <row r="1415" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1415" s="6"/>
+    </row>
+    <row r="1416" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1416" s="6"/>
+    </row>
+    <row r="1417" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1417" s="6"/>
+    </row>
+    <row r="1418" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1418" s="6"/>
+    </row>
+    <row r="1419" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1419" s="6"/>
+    </row>
+    <row r="1420" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1420" s="6"/>
+    </row>
+    <row r="1421" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1421" s="6"/>
+    </row>
+    <row r="1422" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1422" s="6"/>
+    </row>
+    <row r="1423" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1423" s="6"/>
+    </row>
+    <row r="1424" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1424" s="6"/>
+    </row>
+    <row r="1425" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1425" s="6"/>
+    </row>
+    <row r="1426" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1426" s="6"/>
+    </row>
+    <row r="1427" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1427" s="6"/>
+    </row>
+    <row r="1428" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1428" s="6"/>
+    </row>
+    <row r="1429" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1429" s="6"/>
+    </row>
+    <row r="1430" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1430" s="6"/>
+    </row>
+    <row r="1431" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1431" s="6"/>
+    </row>
+    <row r="1432" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1432" s="6"/>
+    </row>
+    <row r="1433" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1433" s="6"/>
+    </row>
+    <row r="1434" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1434" s="6"/>
+    </row>
+    <row r="1435" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1435" s="6"/>
+    </row>
+    <row r="1436" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1436" s="6"/>
+    </row>
+    <row r="1437" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1437" s="6"/>
+    </row>
+    <row r="1438" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1438" s="6"/>
+    </row>
+    <row r="1439" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1439" s="6"/>
+    </row>
+    <row r="1440" spans="15:15" ht="24.95" customHeight="1">
+      <c r="O1440" s="6"/>
+    </row>
   </sheetData>
-  <autoFilter ref="O1:O1117" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="O1:O1143" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -9212,7 +9837,7 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>21</v>
@@ -9237,7 +9862,7 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="2" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>21</v>
@@ -9287,7 +9912,7 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>21</v>
@@ -9312,7 +9937,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>21</v>
@@ -9537,7 +10162,7 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="2" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>21</v>
@@ -9555,7 +10180,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="3" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
@@ -9637,7 +10262,7 @@
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="2" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>21</v>
@@ -10263,7 +10888,7 @@
     </row>
     <row r="79" spans="1:17">
       <c r="A79" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>21</v>
@@ -10274,7 +10899,7 @@
     </row>
     <row r="80" spans="1:17">
       <c r="A80" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>21</v>
@@ -10285,7 +10910,7 @@
     </row>
     <row r="81" spans="1:19">
       <c r="A81" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>21</v>

</xml_diff>